<commit_message>
adds examples, generates HTML page for examples
- examples have been revised for v2 (RDF files)
- index of examples has been updated (in UCR spreadsheet)
- HTML index page shows list of all examples
- macro example_aside has been updated to insert examples in other pages
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="205">
   <si>
     <t>ID</t>
   </si>
@@ -157,10 +157,12 @@
     <t>E0001</t>
   </si>
   <si>
-    <t>Dummy Example 1</t>
-  </si>
-  <si>
-    <t>Dummy Example description</t>
+    <t>Implications of using SKOS vs OWL</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example highlights the implications of using DPV with RDFS+SKOS and OWL semantics. The RDFS+SKOS model is suitable for when DPV concepts have to be used 'directly' e.g. an use-case wants to use 'Encryption' from DPV as a technical measure without creating a specific 'instance' representing their implementation of the encryption. RDFS+SKOS model is also suitable for when an use-case wants to further create an hierarchical taxonomy of the different 'Encryption' concepts they are using. Such use of DPV concepts covers both T-box and A-box, and does not restrict or require the underlying ontology/schema to be constantly changed as new concepts are identified in an use-case.&lt;/p&gt;
+      &lt;p&gt;In comparison, the OWL2 model defines concepts as classes and instances with a clear separation between the two i.e. the Tbox and Abox are separate. This means the concept 'Encryption' cannot be directly used with OWL2 semantics and an instance of it must first be created. If instead DPV had provided 'Encryption' as an instance (of Technical Measure) then the further expansion and creation of a hierarchy of encryption concepts described earlier is not feasible in OWL2 as it results in a complex graph which is not efficient for reasoning. Further, making changes such as promoting 'Encryption' from instance to class requires changing the ontology/schema - which may not always be possible or feasible in use-cases.&lt;/p&gt;
+      &lt;p&gt;Thus, the relative strengths and weaknesses of RDFS+SKOS and OWL2 serialisations dictate which should be used. RDFS+SKOS is 'lightweight' and better if the use-case only requires rudimentary or simple reasoning. OWL2 is  better suited for semantic reasoners that can perform complex discovery and validation processes but require more strict and restricted use of concepts. By providing both serialisations, DPV enables the adopters to choose the most suitable serialisation that supports their use-case and/or existing implementations, and retains semantic interoperability based on converting between SKOS and OWL2 (see &lt;a href="https://www.w3.org/2006/07/SWD/SKOS/skos-and-owl/master.html"&gt;Using OWL and SKOS (2008)&lt;/a&gt;).&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0001.ttl</t>
@@ -172,43 +174,50 @@
     <t>file</t>
   </si>
   <si>
+    <t>dpv:</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit</t>
+  </si>
+  <si>
+    <t>E0002</t>
+  </si>
+  <si>
+    <t>Extending concepts to represent use-case specific information</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;DPV defines the (broad) concept of &lt;a href="https://w3id.org/dpv#Marketing"&gt;&lt;code&gt;Marketing&lt;/code&gt;&lt;/a&gt; in its &lt;code&gt;Purpose&lt;/code&gt; hierarchy to represent information about (purposes related to) marketing activities and topics. For a use-case which requires representing purposes (note: plural) related to &lt;i&gt;marketing of new products&lt;/i&gt;, the broad &lt;code&gt;Marketing&lt;/code&gt; concept is extended as a &lt;i&gt;child&lt;/i&gt; or &lt;i&gt;subclass&lt;/i&gt; concept for representing the intended purpose as, e.g. &lt;code&gt;MarketingNewProducts&lt;/code&gt;.&lt;/p&gt;
+      &lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; Here the prefix &lt;code&gt;ex:&lt;/code&gt; represents &lt;code&gt;http://example.com#&lt;/code&gt; - which is a convention for representing additional examples or concepts, such as those created as part of the use-case. The rest of the document follows this nomenclature and convention.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0002.ttl</t>
+  </si>
+  <si>
+    <t>E0003</t>
+  </si>
+  <si>
+    <t>Extending multiple concepts</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;For example, two TV companies (&lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt;) extend the concept &lt;code&gt;Optimisation&lt;/code&gt; to reflect their respective purposes. When exchanging information about their use-cases with each other (or with a third party), by following the chain of use-case specific concepts it is possible to deduce that both &lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt; are doing optimisations for consumers. Thus a common language or interface can be developed based on using DPV as a point of interoperability and commonality which can be used by adopters to define the specifics of their use-case. For example, in the above use-case, a common notice generation algorithm could be created and used to inform users of both services the purposes each company is using data for.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0003.ttl</t>
+  </si>
+  <si>
     <t>dpv:Purpose</t>
   </si>
   <si>
-    <t>accepted</t>
-  </si>
-  <si>
-    <t>Harshvardhan J. Pandit</t>
-  </si>
-  <si>
-    <t>E0002</t>
-  </si>
-  <si>
-    <t>Dummy Example 2</t>
-  </si>
-  <si>
-    <t>Dummy Example 2 description</t>
-  </si>
-  <si>
-    <t>E0002.ttl</t>
-  </si>
-  <si>
-    <t>E0003</t>
-  </si>
-  <si>
-    <t>Extending Purpose for Use-Case</t>
-  </si>
-  <si>
-    <t>DPV defines the (broad) concept Marketing in its Purpose hierarchy to represent information about (purposes related to) marketing activities and topics. For a use-case which requires representing purposes (note: plural) related to marketing of new products, the broad Marketing concept is extended as a child or subclass concept for representing the intended purpose as, e.g. MarketingNewProducts.</t>
-  </si>
-  <si>
-    <t>E0003.ttl</t>
-  </si>
-  <si>
     <t>E0004</t>
   </si>
   <si>
-    <t>DPV-OWL: Extending Purpose for Use-Case</t>
+    <t>Interoperability of extended concepts across use-cases</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;For example, two TV companies (&lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt;) extend the concept &lt;code&gt;Optimisation&lt;/code&gt; to reflect their respective purposes as follows:&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0004.ttl</t>
@@ -217,25 +226,25 @@
     <t>E0005</t>
   </si>
   <si>
-    <t>Combining concepts to indicate they always occur together</t>
-  </si>
-  <si>
-    <t>Consider the use-case where an activity simultaneously uses the data while collecting it. The first representation (&lt;code&gt;ActivityA&lt;/code&gt;) models them separately - which is not accurate as it is ambiguous in terms of collection and usage taking place independently. By extending the collect and use concepts to create a new concept called &lt;code&gt;CollectAndUse&lt;/code&gt;, it is possible to accurately declare that they both occur as a concurrent operation. Such combinations of concepts are also useful to collectively represent or annotate additional information such as: technologies involved, implementation details, or agents involved</t>
+    <t>Process used to combine core concepts and represent an use-case</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;An example of how &lt;code&gt;Process&lt;/code&gt; brings together the core concepts, consider the example where &lt;code&gt;Acme&lt;/code&gt; is a &lt;code&gt;DataController&lt;/code&gt; that &lt;code&gt;Collect&lt;/code&gt;(s) and &lt;code&gt;Use&lt;/code&gt;(s) &lt;code&gt;Email&lt;/code&gt; for &lt;code&gt;ServiceProvision&lt;/code&gt;. Note that the &lt;code&gt;pd:EmailAddress&lt;/code&gt; is a concept from the [[[PD]]] extension.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0005.ttl</t>
   </si>
   <si>
-    <t>dpv:Processing</t>
+    <t>dpv:Process</t>
   </si>
   <si>
     <t>E0006</t>
   </si>
   <si>
-    <t>Maintaining Interoperability between Use-Cases</t>
-  </si>
-  <si>
-    <t>For example, two TV companies (&lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt;) extend the concept &lt;code&gt;Optimisation&lt;/code&gt; to reflect their respective purposes. When exchanging information about their use-cases with each other (or with a third party), by following the chain of use-case specific concepts it is possible to deduce that both &lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt; are doing optimisations for consumers. Thus a common language or interface can be developed based on using DPV as a point of interoperability and commonality which can be used by adopters to define the specifics of their use-case. For example, in the above use-case, a common notice generation algorithm could be created and used to inform users of both services the purposes each company is using data for.</t>
+    <t>Nesting Processes</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Consider the example where &lt;em&gt;Acme&lt;/em&gt;, as a &lt;em&gt;DataController&lt;/em&gt;, maintains records of its processing activities using &lt;code&gt;Process&lt;/code&gt; to represent one of its services. In this, it collects email, uses it for internal analyses based on &lt;em&gt;Legitimate Interests&lt;/em&gt;, and also sends marketing information by using a processor based on the data subject's consent. Using nesting of processes, the information can be expressed at a granular level representing service, individual purposes, and so on.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0006.ttl</t>
@@ -244,25 +253,22 @@
     <t>E0007</t>
   </si>
   <si>
-    <t>Use of PersonalDataHandling to group how data is being processed</t>
-  </si>
-  <si>
-    <t>For an example of how &lt;code&gt;PersonalDataHandling&lt;/code&gt; brings together the core concepts, consider the example where &lt;code&gt;Acme&lt;/code&gt; is a &lt;code&gt;DataController&lt;/code&gt; that &lt;code&gt;Collect&lt;/code&gt;(s) and &lt;code&gt;Use&lt;/code&gt;(s) &lt;code&gt;Email&lt;/code&gt; for &lt;code&gt;ServiceProvision&lt;/code&gt;.</t>
+    <t>Extending Purposes and adding human-readable descriptions</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, a new purpose is created by extending &lt;code&gt;dpv:FraudPreventionAndDetection&lt;/code&gt; and annotated with human-readable information. The interpretation of this purpose is thus more clear in relation to how it is applied or used within that use-case, and also serves to compare it with other purposes within the same category.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0007.ttl</t>
   </si>
   <si>
-    <t>dpv:PersonalDataHandling</t>
-  </si>
-  <si>
     <t>E0008</t>
   </si>
   <si>
-    <t>Nesting PersonalDataHandling for modular expression of processing operations</t>
-  </si>
-  <si>
-    <t>onsider the example where &lt;em&gt;Acme&lt;/em&gt;, as a &lt;em&gt;DataController&lt;/em&gt;, maintains records of its processing activities using &lt;code&gt;PersonalDataHandling&lt;/code&gt; to represent one of its services. In this, it collects email, uses it for internal analyses based on &lt;em&gt;LegitimateInterests&lt;/em&gt;, and also sends marketing information by using a processor based on the data subject's consent. Using nesting of personal data handling, the information can be expressed at granular level representing service, individual purposes, and so on.</t>
+    <t>Using NACE codes to restrict Purposes</t>
+  </si>
+  <si>
+    <t>For example, the following purpose concerns implementing access control with the domain specified as scientific research using its corresponding NACE code &lt;code&gt;M72&lt;/code&gt; to indicate sectorial implications for what "access control" and "enforce security" are expected to imply.</t>
   </si>
   <si>
     <t>E0008.ttl</t>
@@ -271,52 +277,58 @@
     <t>E0009</t>
   </si>
   <si>
-    <t>Adding human-readable descriptions</t>
-  </si>
-  <si>
-    <t>In this example, a new purpose is created by extending &lt;code&gt;dpv:FraudPreventionAndDetection&lt;/code&gt; and annotated with human-readable information. The interpretation of this purpose is thus more clear in relation to how it is applied or used within that use-case, and also serves to compare it with other purposes within the same category.</t>
+    <t>Derivation and inference of personal data</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This use-case collects browser fingerprint and IP Address to identify the country one is visiting from, and to infer language to be used for personalisation. Note that this example uses [[PD]] for personal data concepts.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0009.ttl</t>
   </si>
   <si>
+    <t>dpv:Derive,dpv:Infer,dpv:DerivedPersonalData,dpv:InferredPersonalData</t>
+  </si>
+  <si>
     <t>E0010</t>
   </si>
   <si>
-    <t>Using NACE codes to restrict Purposes</t>
-  </si>
-  <si>
-    <t>For example, the following purpose concerns implementing access control with the domain specified as scientific research using its corresponding NACE code &lt;code&gt;M72&lt;/code&gt; to indicate sectorial implications for what "access control" and "enforce security" are expected to imply.</t>
+    <t>Indicating personal data is sensitive or special category</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In a medical study involving genetic data, the person's collected blood samples are considered to be 'special category' personal data under the GDPR. In addition to this, the person's identifier associated with that dataset to enable monitoring future appointments is considered sensitive within the medical centre. Note that the examples use the [[PD]] extension to represent some concepts.&lt;/p&gt;
+        &lt;p&gt;In this example, the knowledge that blood samples are of type 'special category' can be inferred from the fact that they are a form of &lt;i&gt;Medical Health&lt;/i&gt; which is a 'special category'. However, the example considers best practices that suggest explicitly identifying and denoting that blood samples are also of type 'special category'.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0010.ttl</t>
   </si>
   <si>
-    <t>dpv:Purpose,dpv:Sector</t>
+    <t>dpv:SensitivePersonalData,dpv:SpecialCategoryPersonalData</t>
   </si>
   <si>
     <t>E0011</t>
   </si>
   <si>
-    <t>Storage Conditions</t>
-  </si>
-  <si>
-    <t>Acme is a Data Processor that stores data within servers located in Ireland for a period of one year.</t>
+    <t>Indicating Storage Conditions</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example includes Acme as a Data Processor that stores data within servers located in Ireland for a period of one year. The temporal information is represented using [[[TIME]]], and the location is specified using [[[LOC]]].&lt;/p&gt;&lt;p&gt;In this example, the &lt;code&gt;StorageCondition&lt;/code&gt; is expressed as a separate policy applicable. It is also possible to directly express it over other concepts such as a service, technology, or a processing operation, e.g. to say &lt;code&gt;ex:AcmeStore dpv:hasStorageCondition ...&lt;/code&gt;.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0011.ttl</t>
   </si>
   <si>
-    <t>dpv:DataProcessor,dpv:Processing,dpv:StorageCondition,dpv:Location,dpv:Duration</t>
+    <t>dpv:StorageCondition</t>
   </si>
   <si>
     <t>E0012</t>
   </si>
   <si>
-    <t>Data Sources</t>
-  </si>
-  <si>
-    <t>Data sources can be the data subject (direct or indirect), the data controller or processor (itself), or another entity (third party). The below example provides an overview of these with distinctions between source and method of generation.</t>
+    <t>Indicating Data Sources</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Data sources can be the data subject (direct or indirect), the data controller or processor (itself), or another entity (third party). The below example provides an overview of these with distinctions between source and method of generation.&lt;/p&gt;
+        &lt;p&gt;In this example, &lt;code&gt;ex:S01&lt;/code&gt; represents direct collection of data from the data subject, while &lt;code&gt;ex:S02&lt;/code&gt; represents indirect collection where data is derived or observed - or undergoes any operation that still points to the data subject as the source. &lt;code&gt;ex:S03&lt;/code&gt; infers data, which means the inferring entity (the Controller in this case) is the source of this data - even if the inferred data is based on data collected from the Data Subject. &lt;code&gt;ex:S04&lt;/code&gt; has data sourced from another entity - such as a Third Party, but could also refer to a Data Processor. &lt;code&gt;ex:S05&lt;/code&gt; represents collection of data from a public dataset that has been published by the data subject themselves.&lt;/p&gt;
+        &lt;p&gt;Note that the above example is illustrative - it may be pertinent to provide documentation about each data source to ensure sufficient information is recorded for intended purposes. For example, the method of collection (e.g. forms), or inference (e.g. algorithm), or public dataset (e.g. link, license).&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0012.ttl</t>
@@ -328,253 +340,284 @@
     <t>E0013</t>
   </si>
   <si>
-    <t>Automated Processing with Human Involvement</t>
-  </si>
-  <si>
-    <t>Consider the use of a spam filter that is based on automated processing operations where humans provide inputs, have oversight of the operation, and results in automated decision making for whether communications should be propogated. A new separate filter is developed that utilises a novel spam detection criteria that also takes into account communications other than emails for the sender and makes automated decisions whether to permit communication to proceed. Such explicit annotation of several high-risk operations assists in performing impact assessments for this technology, as well as understanding the extent and effectiveness of human involvement to mitigate risks and issues.</t>
+    <t>Spam filter as Automated Decision Making with Human Involvement</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Consider the use of a spam filter that is based on automated processing operations where humans provide inputs, have oversight of the operation, and results in automated decision making for whether communications should be propagated. A new separate filter is developed that utilises a novel spam detection criteria that also takes into account communications other than emails for the sender and makes automated decisions whether to permit communication to proceed. Such explicit annotation of several high-risk operations assists in performing impact assessments for this technology, as well as understanding the extent and effectiveness of human involvement to mitigate risks and issues.&lt;/p&gt;
+        &lt;p&gt;In this example, the Spam Filter process allows the users to reverse the effects (i.e. emails marked as spam) but does not allow opting out from the process (i.e. stop spam filtering). The spam detection algorithm performs automated decision making (by deciding which emails to accept), systemic monitoring (of communications), and evaluation and scoring (by scoring contents of emails and senders/recipients). The spam detection algorithm also indicates what human involvement is expected - to provide input (e.g. mark emails as spam) and intervention (e.g. change spam criterias).&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0013.ttl</t>
   </si>
   <si>
-    <t>dpv:Automation</t>
+    <t>dpv:AutomationLevel,dpv:HumanInvolvement</t>
   </si>
   <si>
     <t>E0014</t>
   </si>
   <si>
-    <t>Derivation and inference of personal data</t>
-  </si>
-  <si>
-    <t>This use-case collects browser fingerprint and IP Address to identify the country one is visiting from, and to infer language to be used for personalisation. Note that this example uses [[DPV-PD]] for personal data concepts.</t>
+    <t>Denoting Legal Basis within a Process</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The &lt;code&gt;LegalBasis&lt;/code&gt; can be associated with any concept using the relation &lt;code&gt;hasLegalBasis&lt;/code&gt;. Such associations are of three types: (1) where the legal basis refers to an instance, such as the consent or contract associated with a particular data subject; (2)  where the legal basis refers to the category that will be used to justify processing, such as the concept &lt;i&gt;consent&lt;/i&gt; to denote consent will be the basis for indicated processing; and lastly (3) where the legal basis is defined with a context, such as &lt;i&gt;consent of service consumers&lt;/i&gt;.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0014.ttl</t>
   </si>
   <si>
-    <t>dpv:Purpose,dpv:Processing,dpv:PersonalDataHandling,dpv:Derive,dpv:Infer</t>
+    <t>dpv:LegalBasis</t>
   </si>
   <si>
     <t>E0015</t>
   </si>
   <si>
-    <t>Indicating personal data is sensitive or special category</t>
-  </si>
-  <si>
-    <t>In this example, the knowledge that blood samples are of type 'special category' can be inferred from the fact that they are a form of &lt;i&gt;Medical Health&lt;/i&gt; which is a 'special category'. However, the example considers best practices that suggest explicitly identifying and denoting that blood samples are also of type 'special category'.</t>
+    <t>Indicating consent as a legal basis</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Here, a process instance represents some context (e.g. a service, or a product, or some operation), and the example specifies that the legal basis for these is the use of consent.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0015.ttl</t>
   </si>
   <si>
-    <t>dpv:SpecialCategoryPersonalData,dpv:SensitivePersonalData</t>
+    <t>dpv:Consent</t>
   </si>
   <si>
     <t>E0016</t>
   </si>
   <si>
-    <t>Protecting data using encryption and access control</t>
-  </si>
-  <si>
-    <t>To indicate data is encrypted using the &lt;a href="https://en.wikipedia.org/wiki/RSA_(cryptosystem)"&gt;Rivest-Shamir-Adleman (RSA) method&lt;/a&gt;, one would extend the &lt;a href="https://www.w3id.org/dpv#Encryption"&gt;&lt;code&gt;Encryption&lt;/code&gt;&lt;/a&gt; concept within DPV to represent &lt;code&gt;RSA&lt;/code&gt;, and then instantiate it with the specific implementation used (e.g. to indicate key size). Access to this data is further restricted by requiring a password or credential.</t>
+    <t>Indicating details about an individual's consent</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, an individual's consent is recorded with abstraction in the form of linking to a common process instance from the previous example. This 'common' process represents processing taking place for all data subjects, whereas the consent instance refers only to the individual with a link to this common information. This is to present an alternative method for storing information as compared to extensive consent records.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0016.ttl</t>
   </si>
   <si>
-    <t>dpv:Encryption,dpv:AccessControlMethod</t>
+    <t>dpv:ConsentRecord</t>
   </si>
   <si>
     <t>E0017</t>
   </si>
   <si>
-    <t>Indicating staff training for use of Credentials</t>
-  </si>
-  <si>
-    <t>To indicate staff are trained in the use of credentials, and that a policy exists regarding this, the use of &lt;code&gt;OrganisationalMeasure&lt;/code&gt; concepts can be combined in several ways. Note that the interpretations for how staff training is associated with credentials, or contains training regarding credentials is arbitrary in notation. It is intended to demonstrate how different perspectives can be represented so as to be suitable to the organisation's documentation practices.</t>
+    <t>Representing notice, provision, expiry, and withdrawal information for consent</t>
+  </si>
+  <si>
+    <t>This example first specifies a privacy notice as a document is being used in the context of a service as represented using a personal data handling instance. Then it provides an alternative representation where the contents of a notice are described using DPV.</t>
   </si>
   <si>
     <t>E0017.ttl</t>
   </si>
   <si>
-    <t>dpv:StaffTraining,dpv:Policy</t>
+    <t>dpv:Notice,dpv:PrivacyNotice</t>
   </si>
   <si>
     <t>E0018</t>
   </si>
   <si>
-    <t>Notice used in an activity</t>
-  </si>
-  <si>
-    <t>This example first specifies a privacy notice as a document is being used in the context of a service as represented using a personal data handling instance. Then it provides an alternative representation where the contents of a notice are described using DPV.</t>
+    <t>Using consent types</t>
+  </si>
+  <si>
+    <t>This example shows use of DPV consent types to distinguish between 'expressed' and 'explicitly expressed' consent</t>
   </si>
   <si>
     <t>E0018.ttl</t>
   </si>
   <si>
-    <t>dpv:PersonalDataHandling,dpv:PrivacyNotice,dpv:ServiceProvision,dpv:Collect</t>
+    <t>dpv:Consent,dpv:ExpressedConsent,dpv:ExplicitlyExpressedConsent</t>
   </si>
   <si>
     <t>E0019</t>
   </si>
   <si>
-    <t>Consent record</t>
-  </si>
-  <si>
-    <t>This example shows a consent record containing the topic of consent (i.e. which processing activities it was about), its current status, and when it was given by the data subject. The structure of a record is highly dependant on the requirements of the use-case, and can vary across implementations. In this case, it is based on a draft of the ISO/IEC AWI TS 27560 Privacy technologies - Consent record information structure.</t>
+    <t>Indicating Entity Information, including DPO and Representatives</t>
+  </si>
+  <si>
+    <t>This example shows how information about representatives can be associated with an entity</t>
   </si>
   <si>
     <t>E0019.ttl</t>
   </si>
   <si>
-    <t>dpv:ConsentRecord,dpv:PersonalDataHandling,dpv:Consent,dpv:DataController,dpv:Jurisdiction,dpv:Recipient,dpv:ConsentStatus,dpv:ConsentType,dpv:Duration</t>
+    <t>dpv:Representative,dpv:DPO</t>
   </si>
   <si>
     <t>E0020</t>
   </si>
   <si>
-    <t>Controller-Processor agreement</t>
-  </si>
-  <si>
-    <t>Acme is the Data Controller, that contracts BetaInc as a Data Processor to analyse raw call logs and provide statistical patterns.</t>
+    <t>Using technical measure: Protecting data using encryption and access control</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To indicate data is encrypted using the &lt;a href="https://en.wikipedia.org/wiki/RSA_(cryptosystem)"&gt;Rivest-Shamir-Adleman (RSA) method&lt;/a&gt;, one would extend the &lt;a href="https://w3id.org/dpv#Encryption"&gt;&lt;code&gt;Encryption&lt;/code&gt;&lt;/a&gt; concept within DPV to represent &lt;code&gt;RSA&lt;/code&gt;, and then instantiate it with the specific implementation used (e.g. to indicate key size). Access to this data is further restricted by requiring a password or credential.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0020.ttl</t>
   </si>
   <si>
-    <t>dpv:DataController,dpv:ControllerProcessor,dpv:ControllerProcessorAgreement,dpv:PersonalDataHandling,dpv:Transfer,dpv:DataSource</t>
+    <t>dpv:TechnicalMeasure,dpv:Encryption,dpv:AccessControlMethod</t>
   </si>
   <si>
     <t>E0021</t>
   </si>
   <si>
+    <t>Using organisational measure: Indicating staff training for use of Credentials</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To indicate staff are trained in the use of credentials, and that a policy exists regarding this, the use of &lt;code&gt;OrganisationalMeasure&lt;/code&gt; concepts can be combined in several ways. Note that the interpretations for how staff training is associated with credentials, or contains training regarding credentials is arbitrary in notation. It is intended to demonstrate how different perspectives can be represented so as to be suitable to the organisation's documentation practices.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0021.ttl</t>
+  </si>
+  <si>
+    <t>dpv:OrganisationalMeasure,dpv:StaffTraining</t>
+  </si>
+  <si>
+    <t>E0022</t>
+  </si>
+  <si>
+    <t>Privacy Notice used in an activity</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example first specifies a privacy notice as a document is being used in the context of a service as represented using a process instance. Then it provides an alternative representation where the contents of a notice are described using DPV.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0022.ttl</t>
+  </si>
+  <si>
+    <t>dpv:PrivacyNotice</t>
+  </si>
+  <si>
+    <t>E0023</t>
+  </si>
+  <si>
+    <t>Consent record example</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This (simplified) example shows a consent record containing the topic of consent (i.e. which processing activities it was about), its current status, and when it was given by the data subject. The structure of a record is highly dependent on the requirements of the use-case, and can vary across implementations. In this case, it is based on the ISO/IEC TS 27560:2023 Privacy technologies — Consent record information structure, for which we provide the implementation guide [[[GUIDE-Consent-27560]]].&lt;/p&gt;&lt;p&gt;The example uses the &lt;a href="https://dublincore.org/specifications/dublin-core/dcmi-terms/"&gt;DCMI Metadata Terms (dct)&lt;/a&gt; vocabulary to indicate metadata such as title and timestamps. Other vocabularies such as &lt;a href="https://www.w3.org/TR/prov-o/"&gt;PROV-O&lt;/a&gt; can be used to also indicate provenance information such as when it was generated and how it was produced.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0023.ttl</t>
+  </si>
+  <si>
+    <t>E0024</t>
+  </si>
+  <si>
+    <t>Controller-Processor agreement denoting processing to be carried out</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Acme is the Data Controller that contracts BetaInc as a Data Processor to analyse raw call logs and provide statistical patterns.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0024.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ControllerProcessorAgreement</t>
+  </si>
+  <si>
+    <t>E0025</t>
+  </si>
+  <si>
     <t>Data transfer safeguards</t>
   </si>
   <si>
-    <t>This example represents a contractual agreement between a controller and a processor indicating the use of encryption and EU commission approved Standard Contractual Clauses as specific measures to safeguard data transfers between them.</t>
-  </si>
-  <si>
-    <t>E0021.ttl</t>
-  </si>
-  <si>
-    <t>dpv:ControllerProcessorAgreement,dpv:DataTransferSafeguard,eu-gdpr:SCCsByCommission</t>
-  </si>
-  <si>
-    <t>E0022</t>
-  </si>
-  <si>
-    <t>Denoting Legal Basis</t>
-  </si>
-  <si>
-    <t>The &lt;code&gt;LegalBasis&lt;/code&gt; can be associated with any concept using the relation &lt;code&gt;hasLegalBasis&lt;/code&gt;. Such associations are of three types: (1) where the legal basis refers to an instance, such as the consent or contract associated with a particular data subject; (2) where the legal basis refers to the category that will be used to justify processing, such as the concept &lt;i&gt;consent&lt;/i&gt; to denote consent will be the basis for indicated processing; and lastly (3) where the legal basis is the denoted with context, such as &lt;i&gt;consent of service consumers&lt;/i&gt;.</t>
-  </si>
-  <si>
-    <t>E0022.ttl</t>
-  </si>
-  <si>
-    <t>dpv:LegalBasis,dpv:PersonalDataHandling,dpv:Consent</t>
-  </si>
-  <si>
-    <t>E0023</t>
-  </si>
-  <si>
-    <t>Consent as legal basis</t>
-  </si>
-  <si>
-    <t>Here, a personal data handling instance represents some context (e.g. a service, or a product, or some opreation), and the example specifies that the legal basis for these is the use of consent.</t>
-  </si>
-  <si>
-    <t>E0023.ttl</t>
-  </si>
-  <si>
-    <t>dpv:LegalBasis,dpv:Consent</t>
-  </si>
-  <si>
-    <t>E0024</t>
-  </si>
-  <si>
-    <t>Details of Consent</t>
-  </si>
-  <si>
-    <t>In this example, an individual's consent is recorded with abstraction in the form of linking to a common personal data handling instance from the previous example. This 'common' personal data handling represents processing taking place for all data subjects, whereas the consent instance refers only to the individual with a link to this common information. This is to present an alternative method for storing information as compared to extensive consent records.</t>
-  </si>
-  <si>
-    <t>E0024.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType</t>
-  </si>
-  <si>
-    <t>E0025</t>
-  </si>
-  <si>
-    <t>Consent Notice</t>
-  </si>
-  <si>
-    <t>Representing notice, provision, expiry, and withdrawal information for consent</t>
+    <t>&lt;p&gt;This example represents a contractual agreement between a controller and a processor indicating the use of encryption and EU commission approved Standard Contractual Clauses as specific measures to safeguard data transfers between them.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0025.ttl</t>
   </si>
   <si>
-    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType,dpv:Notice,dpv:PrivacyNotice</t>
+    <t>dpv:DataTransferSafeguard</t>
   </si>
   <si>
     <t>E0026</t>
   </si>
   <si>
-    <t>Using consent types</t>
-  </si>
-  <si>
-    <t>Expressing consent type is required as legal basis and as instances</t>
+    <t>Example of Contextual Necessity</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, a &lt;code&gt;Process&lt;/code&gt; instance consists of two nested &lt;code&gt;Process&lt;/code&gt; instances for each of the optional and required parts. The personal data category 'Account Identifier' is indicated as being required for 'Communication for Customer Care', while the use of 'Email' is optional for the same purpose.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0026.ttl</t>
   </si>
   <si>
+    <t>dpv:Necessity</t>
+  </si>
+  <si>
     <t>E0027</t>
   </si>
   <si>
-    <t>Describing Entities</t>
-  </si>
-  <si>
-    <t>Indicating Entity Information, including DPO and Representatives</t>
+    <t>Indicating risks, consequences, and impacts</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, we consider &lt;i&gt;Risk&lt;/i&gt; can be associated with any  concept given its broad existence and applicability, and that its mitigation is a technical and organisational measure. Using this, the implemented or adopted technical and organisational measures within an use-case are annotated with the risks they address or mitigate, along with specific impacts that may occur if the risk were to occur. For example, the storage of personal data within a database has an implementation of access control that mitigates the consequence of unauthorised access and its impact to cause harm.&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0027.ttl</t>
   </si>
   <si>
-    <t>dpv:Entity</t>
+    <t>dpv:Risk,dpv:Consequence,dpv:Impact</t>
   </si>
   <si>
     <t>E0028</t>
   </si>
   <si>
-    <t>Contextual Necessity</t>
-  </si>
-  <si>
-    <t>In this example, a &lt;code&gt;PersonalDataHandling&lt;/code&gt; instance is comprised of two nested &lt;code&gt;PersonalDataHandling&lt;/code&gt; instances for each of the optional and required parts. The personal data category 'Account Identifier' is indicated as being required for 'Communication for Customer Care', while the use of 'Email' is optional for the same purpose.</t>
+    <t>Rule specifying permission</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, a Process which consists of using an email address for service provision using the legal basis as Consent is permitted&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0028.ttl</t>
   </si>
   <si>
-    <t>dpv:Context,dpv:Necessity,dpv:PersonalDataHandling</t>
+    <t>dpv:Permission</t>
   </si>
   <si>
     <t>E0029</t>
   </si>
   <si>
-    <t>Risk and Consequence</t>
-  </si>
-  <si>
-    <t>In this example, we consider &lt;i&gt;Risk&lt;/i&gt; can be associated with any concept given its broad existence and applicability, and that its mitigation is a technical and organisational measure. Using this, the implemented or adopted technical and organisational measures within an use-case are annotated with the risks they address or mitigate, along with specific impacts that may occur if the risk were to occur. For example, the storage of personal data within a database has an implementation of access control that mitigates the consequence of unauthorised access and its impact to cause harm.</t>
+    <t>Rule specifying prohibition</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, the hasProhibition relation is directly used to assert a prohibition to handle Health data within a Process:&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0029.ttl</t>
   </si>
   <si>
-    <t>dpv:Risk,dpv:Consequence,dpv:Impact,dpv:Harm,dpv:RiskMitigationMeasure</t>
+    <t>dpv:Prohibition</t>
+  </si>
+  <si>
+    <t>E0030</t>
+  </si>
+  <si>
+    <t>Rule combining DPV with ODRL</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this example, DPV is complemented with ODRL, following the ODRL implementation best practices, to assert an obligation to Anonymise data in order to use it:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0030.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Rule</t>
+  </si>
+  <si>
+    <t>E0031</t>
+  </si>
+  <si>
+    <t>Using Service to group related processes</t>
+  </si>
+  <si>
+    <t>This example shows the use of Service concept to represent a 'service' provided by an organisation, which includes two processes for data collection and service provision</t>
+  </si>
+  <si>
+    <t>E0031.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Service,dpv:Process</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -602,7 +645,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -636,10 +679,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="&quot;Arial&quot;"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -655,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -676,13 +715,10 @@
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1250,7 +1286,7 @@
         <v>53</v>
       </c>
       <c r="J2" s="6">
-        <v>44846.0</v>
+        <v>45453.0</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>54</v>
@@ -1300,7 +1336,7 @@
         <v>53</v>
       </c>
       <c r="J3" s="6">
-        <v>44846.0</v>
+        <v>45453.0</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>54</v>
@@ -1343,873 +1379,937 @@
         <v>51</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="8">
-        <v>44847.0</v>
+      <c r="J4" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="10">
-        <v>44847.0</v>
+      <c r="J5" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>69</v>
       </c>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="E6" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="9"/>
+      <c r="G6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="8">
-        <v>44847.0</v>
+      <c r="J6" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="10">
-        <v>44847.0</v>
+      <c r="J7" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="9"/>
+      <c r="G8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="8">
-        <v>44847.0</v>
+      <c r="J8" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="D9" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="9"/>
+      <c r="G9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="10">
-        <v>44847.0</v>
+      <c r="J9" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>87</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="E10" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="9"/>
+      <c r="G10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="8">
-        <v>44847.0</v>
+      <c r="J10" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="C11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="E11" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="9"/>
+      <c r="G11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="10">
-        <v>44847.0</v>
+      <c r="J11" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>96</v>
       </c>
+      <c r="C12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" s="9"/>
+      <c r="G12" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="8">
-        <v>44847.0</v>
+      <c r="J12" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>101</v>
       </c>
+      <c r="C13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="9"/>
+      <c r="G13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="10">
-        <v>44847.0</v>
+      <c r="J13" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>106</v>
       </c>
+      <c r="C14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="9"/>
+      <c r="G14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="8">
-        <v>44847.0</v>
+      <c r="J14" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>111</v>
       </c>
+      <c r="C15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="9"/>
+      <c r="G15" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="10">
-        <v>44847.0</v>
+      <c r="J15" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="C16" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="E16" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" s="9"/>
+      <c r="G16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="8"/>
       <c r="I16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="8">
-        <v>44847.0</v>
+      <c r="J16" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>121</v>
       </c>
+      <c r="C17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="H17" s="9"/>
+      <c r="G17" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="10">
-        <v>44847.0</v>
+      <c r="J17" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="8">
-        <v>44847.0</v>
+      <c r="J24" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>161</v>
       </c>
+      <c r="D25" s="8" t="s">
+        <v>162</v>
+      </c>
       <c r="E25" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H25" s="9"/>
+      <c r="G25" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="10">
-        <v>44847.0</v>
+      <c r="J25" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>166</v>
       </c>
+      <c r="D26" s="8" t="s">
+        <v>167</v>
+      </c>
       <c r="E26" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="H26" s="9"/>
+      <c r="G26" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J26" s="8">
-        <v>44847.0</v>
+      <c r="J26" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>171</v>
       </c>
+      <c r="D27" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="E27" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H27" s="9"/>
+      <c r="G27" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="10">
-        <v>44847.0</v>
+      <c r="J27" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>175</v>
       </c>
+      <c r="C28" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>177</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="9"/>
+      <c r="G28" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" s="8"/>
       <c r="I28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="8">
-        <v>44847.0</v>
+      <c r="J28" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>180</v>
       </c>
+      <c r="C29" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="E29" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="H29" s="9"/>
+      <c r="G29" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="H29" s="8"/>
       <c r="I29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="10">
-        <v>44847.0</v>
+      <c r="J29" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>185</v>
       </c>
+      <c r="C30" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="E30" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H30" s="9"/>
+      <c r="G30" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J30" s="8">
-        <v>44847.0</v>
+      <c r="J30" s="6">
+        <v>45453.0</v>
       </c>
       <c r="K30" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="6">
+        <v>45453.0</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="9">
+        <v>45453.0</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2230,22 +2330,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation for modules data, processing context
- adds documentation for DPV module data and personal data
- adds documentation for DPV module processing context
- fixes incorrect link to processing context page in DPV spec
- adds examples for data and processing context
- adds concept for Contextually Anonymised Data required for
  anonymisation which is not complete or is only contextual
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="293">
   <si>
     <t>ID</t>
   </si>
@@ -795,6 +795,93 @@
   </si>
   <si>
     <t>dpv:Purpose,dpv:Sector</t>
+  </si>
+  <si>
+    <t>E0044</t>
+  </si>
+  <si>
+    <t>Specifying personal data</t>
+  </si>
+  <si>
+    <t>This example shows how personal data can be specified by for a work email address in four methods: (1) by using the PD taxonomy, (2) extending a concept from PD taxonomy,(3) specifying the exact value of email address, and (4) using external vocabularies such as schema.org. In all of these, it is strongly recommended to include a DPV concept (i.e. declare it as Personal Data) for interoperability, and to align it with the DPV and PD taxonomies where relevant (e.g. to mention it is an email address, or to specify it is identifier, or that it is sensitive - which it is not in this case)</t>
+  </si>
+  <si>
+    <t>E0044.ttl</t>
+  </si>
+  <si>
+    <t>dpv:PersonalData,dpv:hasPersonalData</t>
+  </si>
+  <si>
+    <t>E0045</t>
+  </si>
+  <si>
+    <t>Indicating data belongs to sensitive or special category</t>
+  </si>
+  <si>
+    <t>This example shows how data can be indicated as being sensitive or belonging to special category. It also shows the use of PD extension which provides a taxonomy of special categories.</t>
+  </si>
+  <si>
+    <t>E0045.ttl</t>
+  </si>
+  <si>
+    <t>E0046</t>
+  </si>
+  <si>
+    <t>Indicating data being collected and derived</t>
+  </si>
+  <si>
+    <t>This example shows a process which first collects email address from the data subject, and then uses it to derive an account identifier. The seeming duplication in information across processing, personal data category, and data source actually represents three distinct concepts - which can be used in various ways for data governance, or legal compliance e.g. to retrieve all data which is collected or to ensure all collected data has a source.</t>
+  </si>
+  <si>
+    <t>E0046.ttl</t>
+  </si>
+  <si>
+    <t>dpv:CollectedPersonalData,dpv:ProvidedPersonalData,dpv:DerivedPersonalData</t>
+  </si>
+  <si>
+    <t>E0047</t>
+  </si>
+  <si>
+    <t>Indicating processing conditions for duration and location</t>
+  </si>
+  <si>
+    <t>This example shows processing conditions where the use (of data or technology) takes place over 6 months and in Ireland (IE) and Netherlands (NL)</t>
+  </si>
+  <si>
+    <t>E0047.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ProcessingCondition,dpv:ProcessingDuration,dpv:ProcessingLocation</t>
+  </si>
+  <si>
+    <t>E0048</t>
+  </si>
+  <si>
+    <t>Indicating storage conditions for duration, location, deletion, and restoration</t>
+  </si>
+  <si>
+    <t>This example shows storage conditions for a 'store' processing operation. It has a duration valid until the event 'account closure' occurs. It has a storage location situated in Ireland (IE) and Netherlands (NL). The deletion occurs 6 months after the event 'account closure'. And restoration is implemented by using (stored) data located in backup systems in Ireland (IE).</t>
+  </si>
+  <si>
+    <t>E0048.ttl</t>
+  </si>
+  <si>
+    <t>dpv:StorageCondition,dpv:StorageDuration,dpv:StorageLocation,dpv:StorageDeletion,dpv:StorageRestoration</t>
+  </si>
+  <si>
+    <t>E0049</t>
+  </si>
+  <si>
+    <t>Indicating data volume, geo-location coverage, data subject scale, and a processing scale</t>
+  </si>
+  <si>
+    <t>This example shows how data volume, data subject scale, and geographic scale can be indicated along with optional information about the exact values involved. It also shows how a qualified scale can be provided as 'processing scale' based on some criteria (not described here).</t>
+  </si>
+  <si>
+    <t>E0049.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ProcessingScale,dpv:GeographicCoverage,dpv:DataVolume,dpv:DataSubjectScale</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -2874,6 +2961,198 @@
         <v>54</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J45" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J46" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J47" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J48" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J50" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2891,22 +3170,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds documentation for DPV context module
- adds documentation with examples for context module in DPV
- adds example to processing DPV module
- adds example to Justifications extension (using the examples macro)
- adds examples
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="363">
   <si>
     <t>ID</t>
   </si>
@@ -882,6 +882,216 @@
   </si>
   <si>
     <t>dpv:ProcessingScale,dpv:GeographicCoverage,dpv:DataVolume,dpv:DataSubjectScale</t>
+  </si>
+  <si>
+    <t>E0050</t>
+  </si>
+  <si>
+    <t>Specifying duration</t>
+  </si>
+  <si>
+    <t>This example shows the various ways in which duration can be expressed - as a period of time (6months), as an end date, or as a fixed number of occurences, or until an event occurs. The example also show some 'bad practices' where the information is expressed directly as strings - and instead shows the benefits of providing semantic information to explicitly indicate what kind of a duration it is which is necessary for unambiguous interpretations.</t>
+  </si>
+  <si>
+    <t>E0050.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Duration,dpv:hasDuration</t>
+  </si>
+  <si>
+    <t>E0051</t>
+  </si>
+  <si>
+    <t>Specifying frequency</t>
+  </si>
+  <si>
+    <t>This example shows the various ways in which frequency can be expressed, including combining frequency with duration to express complex information such as once per day for 6 months</t>
+  </si>
+  <si>
+    <t>E0051.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Frequency,dpv:hasFrequency</t>
+  </si>
+  <si>
+    <t>E0052</t>
+  </si>
+  <si>
+    <t>Specifying necessity and importance in context</t>
+  </si>
+  <si>
+    <t>This example shows a process where email address is required to be collected, and name can be optionally collected. Note that the necessity applies to the entire process i.e. both personal data and the collect processing operation. It also provides an indication of the importance of the process - for example to indicate which processes are important for the organisation (primary importance) and which are not as important or are not crucial (secondary importance).</t>
+  </si>
+  <si>
+    <t>E0052.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Necessity,dpv:hasNecessity</t>
+  </si>
+  <si>
+    <t>E0053</t>
+  </si>
+  <si>
+    <t>Specifying applicability of information</t>
+  </si>
+  <si>
+    <t>This example show how the unavailability, or non-applicability, or unknown applicability of information can be expressed using the Applicability concepts. Note that such situations may represent risks or issues that may require additional attention e.g. where the information is unknown, further steps should be taken to determine the exact applicability.</t>
+  </si>
+  <si>
+    <t>E0053.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Applicability,dpv:hasApplicability</t>
+  </si>
+  <si>
+    <t>E0054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifying status associated with activities </t>
+  </si>
+  <si>
+    <t>This example shows two processes as 'activities' with the status as ongoing and proposed. The proposed activity can be useful to get an audit or approval or indicate future plans.</t>
+  </si>
+  <si>
+    <t>E0054.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ActivityStatus,dpv:hasActivityStatus</t>
+  </si>
+  <si>
+    <t>E0055</t>
+  </si>
+  <si>
+    <t>Specifying compliance status and lawfulness</t>
+  </si>
+  <si>
+    <t>This example shows the compliance status associated with activities in terms of the organisation's policies and for the EU GDPR obligations. It shows how compliance issues and lawfulness can be documented as a status associated with a process. For GDPR, it uses the concepts from EU-GDPR extension regarding lawfulness.</t>
+  </si>
+  <si>
+    <t>E0055.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ComplianceStatus,dpv:hasComplianceStatus,eu-gdpr:GDPRLawfulness</t>
+  </si>
+  <si>
+    <t>E0056</t>
+  </si>
+  <si>
+    <t>Specifying the audit status assocaited with a DPIA</t>
+  </si>
+  <si>
+    <t>This example shows how a DPIA can be documented as an audit - including a status that indicates audit is needed, and maintaining logs for how the DPIA was approved.</t>
+  </si>
+  <si>
+    <t>E0056.ttl</t>
+  </si>
+  <si>
+    <t>dpv:DPIA,dpv:AuditStatus,dpv:hasAuditStatus</t>
+  </si>
+  <si>
+    <t>E0057</t>
+  </si>
+  <si>
+    <t>Expressing GDPR Right to Data Portability could not be fulfilled due to Identity Verification failure</t>
+  </si>
+  <si>
+    <t>The following example describes a GDPR Article 20 Data Portability request not being fulfilled due to identity verification failure. The dpv:RequestRequiresAction concept indicates further action is required - specifically to provide identity documents.</t>
+  </si>
+  <si>
+    <t>E0057.ttl</t>
+  </si>
+  <si>
+    <t>dpv:RightExerciseRecord,dpv:AuditStatus,dpv:hasAuditStatus,dpv:Justification,dpv:hasJustification</t>
+  </si>
+  <si>
+    <t>E0058</t>
+  </si>
+  <si>
+    <t>Expressing a right exercise request is delayed due to high volume of requests</t>
+  </si>
+  <si>
+    <t>The following example uses the justification HighVolumeOfProcesses to represent a high volume of similar processes or requests causing a delay in fulfilling the rights request. The concept dpv:hasDuration is used to indicate the duration of the delay.</t>
+  </si>
+  <si>
+    <t>E0058.ttl</t>
+  </si>
+  <si>
+    <t>dpv:RightNonFulfilmentNotice,dpv:RequestActionDelayed,dpv:Justification,dpv:hasJustification</t>
+  </si>
+  <si>
+    <t>E0059</t>
+  </si>
+  <si>
+    <t>Exercising the right to rectification with contesting accuracy of information as justification</t>
+  </si>
+  <si>
+    <t>The following example shows the justification ContestAccuracy representing contesting the accuracy of information or process to justify why the right to rectification as per GDPR Article 16 is being exercised. The information in question is represented using dpv:hasPersonalData, with two processes indicating which data should be deleted and the correction.</t>
+  </si>
+  <si>
+    <t>E0059.ttl</t>
+  </si>
+  <si>
+    <t>dpv:RightExerciseActivity,dpv:Justification,dpv:hasJustification</t>
+  </si>
+  <si>
+    <t>E0060</t>
+  </si>
+  <si>
+    <t>Specifying the location of a process</t>
+  </si>
+  <si>
+    <t>The following example shows the use of LOC extension to express the location of a process. It also shows how the location fixture and locality concepts are useful to indicate information such as data will be stored locally and shared to a remote cloud server.</t>
+  </si>
+  <si>
+    <t>E0060.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Location,dpv:LocationFixture,dpv:LocationLocality,dpv:hasLocation</t>
+  </si>
+  <si>
+    <t>E0061</t>
+  </si>
+  <si>
+    <t>Associating justifications with right exercise non-fulfilment</t>
+  </si>
+  <si>
+    <t>The following example represents a notice outlining a failure to complete a GDPR Data Portability request due to identity verification failure.</t>
+  </si>
+  <si>
+    <t>E0061.ttl</t>
+  </si>
+  <si>
+    <t>dpv:hasJustification,dpv:Justification,dpv:RightNonFulfilmentNotice,dpv:hasRight</t>
+  </si>
+  <si>
+    <t>E0062</t>
+  </si>
+  <si>
+    <t>Using justifications across categories</t>
+  </si>
+  <si>
+    <t>The justification concept ComplexityOfProcess represents a reason to delay a process due to the complexity of fulfilling it. To instead use it as a justification for not fulfilling the process, we create a new justification that combines the complexity of process and non-fulfilment categories.</t>
+  </si>
+  <si>
+    <t>E0062.ttl</t>
+  </si>
+  <si>
+    <t>dpv:hasJustification,dpv:Justification</t>
+  </si>
+  <si>
+    <t>E0063</t>
+  </si>
+  <si>
+    <t>Expressing data breach notifications to data subjects are not required using a justification</t>
+  </si>
+  <si>
+    <t>The justification RightsFreedomsImpactUnlikely represents an unlikely impact on rights and freedoms, which can be used as a justification to not provide data subjects with a notification about a data breach involving their personal data as per GDPR Article 35-3b.</t>
+  </si>
+  <si>
+    <t>E0063.ttl</t>
+  </si>
+  <si>
+    <t>dpv:hasJustification,dpv:Justification,risk:DataBreachReport</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -3153,6 +3363,454 @@
         <v>54</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J51" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J52" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J53" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J54" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J55" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J56" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J57" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J58" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J59" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J60" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J61" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J62" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J63" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J64" s="9">
+        <v>45454.0</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3170,22 +3828,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>287</v>
+        <v>357</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>289</v>
+        <v>359</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>290</v>
+        <v>360</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>291</v>
+        <v>361</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>292</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds documentation for TOM module in DPV
- adds documentation for DPV TOM module
- adds examples
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="368">
   <si>
     <t>ID</t>
   </si>
@@ -1092,6 +1092,21 @@
   </si>
   <si>
     <t>dpv:hasJustification,dpv:Justification,risk:DataBreachReport</t>
+  </si>
+  <si>
+    <t>E0064</t>
+  </si>
+  <si>
+    <t>Indicating use of a technical measure and its implementation</t>
+  </si>
+  <si>
+    <t>This example specifies a technical measure (access control) being used and specifies that it is implemented by using the database software. It also shows how technologies can have technical measures implemented as part of the system, and also how technologies can indicate they have the capability to provide technical measures for other activities.</t>
+  </si>
+  <si>
+    <t>E0064.ttl</t>
+  </si>
+  <si>
+    <t>dpv:TechnicalMeasure,dpv:hasTechnicalMeasure,dpv:isImplementedUsingTechnology,tech:Capability,tech:hasCapability</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -3811,6 +3826,38 @@
         <v>54</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J65" s="9">
+        <v>45455.0</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3828,22 +3875,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds documentation for rules module in DPV
- adds documentation for rules module in DPV
- adds examples
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="378">
   <si>
     <t>ID</t>
   </si>
@@ -1122,6 +1122,21 @@
   </si>
   <si>
     <t>dpv:LegitimateInterest,dpv:LegitimateInterestOfController</t>
+  </si>
+  <si>
+    <t>E0066</t>
+  </si>
+  <si>
+    <t>Specifying permissions and prohibitions</t>
+  </si>
+  <si>
+    <t>This example show a process where service provision based on consent is permitted, and profiling based on legitimate interest is prohibited</t>
+  </si>
+  <si>
+    <t>E0066.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Permission,dpv:Prohibition,dpv:hasPermission,dpv:hasProhibition</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -3905,6 +3920,38 @@
         <v>54</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J67" s="9">
+        <v>45457.0</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3922,22 +3969,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds documentation for risk module in DPV
- adds documentation for risk module in DPV
- adds examples
- adds examples from RISK page (refactored example aside in HTML)
- adds concept ResidualRisk to DPV risk module, changes the domain/range
  of risk properties associated with residual risks
- removes consequence and impact taxonomy concepts as they have been
  moved to the RISK extension
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="403">
   <si>
     <t>ID</t>
   </si>
@@ -1152,6 +1152,66 @@
   </si>
   <si>
     <t>dpv:Right,dpv:hasRight</t>
+  </si>
+  <si>
+    <t>E0068</t>
+  </si>
+  <si>
+    <t>Using DPV and RISK extension to represent risks</t>
+  </si>
+  <si>
+    <t>This example shows the use of risk concepts in DPV and RISK extension to represent a risk of data breach associated with a process along with its potential consequences and impacts on the data subject. The scenario consists of a risk of data breach with high likelihood and severity, and whose potential consequence includes a loss of data which can lead to financial loss for the data controller and misuse of breached information to cause identity fraud for the data subject. The risk has a mitigation measure, which is to secure the data using the encryption. The residual risk if this measure is applied is shown to have a lower risk level.</t>
+  </si>
+  <si>
+    <t>E0068.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Risk,dpv:hasRisk,dpv:Consequence,dpv:hasConsequence,dpv:Impact,dpv:hasImpact,dpv:Likelihood,dpv:hasLikelihood,dpv:Severity,dpv:hasSeverity,dpv:RiskLevel,dpv:hasRiskLevel,dpv:RiskMitigationMeasure,dpv:isMitigatedByMeasure,dpv:hasImpactOn,dpv:ResidualRisk,dpv:hasResidualRisk</t>
+  </si>
+  <si>
+    <t>E0069</t>
+  </si>
+  <si>
+    <t>Using DPV and RISK extension to represent incidents</t>
+  </si>
+  <si>
+    <t>This example shows the use of incident concepts in DPV and RISK extension to represent a data breach incident along with its potential and actual (i.e. occured) consequences and impacts on the data subject. It shows the consequences of the incident as loss of data, and which is being misused to cause identity fraud. It also refers to the further risk of financial loss, and associates the incident with a previously identified risk (not elaborated in this example). Note that incident details such as timestamps and durations are not shown in this example.</t>
+  </si>
+  <si>
+    <t>E0069.ttl</t>
+  </si>
+  <si>
+    <t>risk:Incident,risk:IncidentStatus,dpv:hasStatus,dpv:Impact,dpv:hasImpact,risk:refersToRisk,risk:DataBreach</t>
+  </si>
+  <si>
+    <t>E0070</t>
+  </si>
+  <si>
+    <t>Indicating personal data involved in an incident</t>
+  </si>
+  <si>
+    <t>This example shows how existing DPV concepts and relations are used to describe what personal data a data breach incident affected and how the data was secured before the incident.</t>
+  </si>
+  <si>
+    <t>E0070.ttl</t>
+  </si>
+  <si>
+    <t>risk:Incident,dpv:hasDuration,dpv:Duration,dpv:hasTechnicalMeasure</t>
+  </si>
+  <si>
+    <t>E0071</t>
+  </si>
+  <si>
+    <t>Using risk controls to express how tech/org measures address the risk</t>
+  </si>
+  <si>
+    <t>In this example, risk controls are used to indicate the technical measure of encryption is used to remove the consequence of misusing the data if it is breached.</t>
+  </si>
+  <si>
+    <t>E0071.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Risk,risk:DataBreach,dpv:hasRiskLevel,dpv:RiskLevel,dpv:hasConsequence,dpv:Consequence,risk:hasRiskControl,risk:RiskControl</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -3999,6 +4059,134 @@
         <v>54</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J69" s="9">
+        <v>45459.0</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J70" s="9">
+        <v>45459.0</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J71" s="9">
+        <v>45459.0</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J72" s="9">
+        <v>45459.0</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4016,22 +4204,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: RiskConcept in RDF, add content to AI, DPV
- Fixes the use of RiskConcept roles in RISK extension, which were
  incorrectly coded to use the extension's namespace rather than always
  using the RISK namespace e.g. `risk:PotentialRisk` if used in AI
  became `ai:PotentialRisk`. Includes RDF and HTML changes.
- DPV rules modules page: Fix missing image fig.1, and Added content,
  example for rule fulfilment status, note on future concepts, and links
  to ODRL in DPV rules module page
- DPV processing module page: added example for expressing processing
  and why to use process. added content for processing categories
  (collect, store, use, erase, share)
- Added content to AI HTML
- Added examples used in above
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="473">
   <si>
     <t>ID</t>
   </si>
@@ -1393,6 +1393,37 @@
   </si>
   <si>
     <t>dpv:VitalInterest,dpv:VitalInterestStatus</t>
+  </si>
+  <si>
+    <t>E0084</t>
+  </si>
+  <si>
+    <t>Stating status of Rule fulfilment</t>
+  </si>
+  <si>
+    <t>This example shows how the status of rules can be expressed in terms of their fulfilment or violation.</t>
+  </si>
+  <si>
+    <t>E0084.ttl</t>
+  </si>
+  <si>
+    <t>dpv:RuleFulfilmentStatus</t>
+  </si>
+  <si>
+    <t>E0085</t>
+  </si>
+  <si>
+    <t>Role of dpv:Processing and using it in dpv:Process</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example shows the myriad ways that processing could be used to describe other non-processing operation information such as personal data and entity involved. To accurately represent the information in a consistent and reusable manner, we recommend using dpv:Process as the way to combine concepts in to a 'unit' and to reuse this in other processes. This means dpv:Processing only specifies information about the processing operation involved, and optionally the technology being used if it is relevant to the context.&lt;/p&gt;
+&lt;p&gt;In Method 1, the processing instance contains personal data and entity involved - this is not recommended as the instance now contains information not related to the processing operation itself. Method 2 shows a processing instance which is implemented using a specific technology. This is acceptable as it describes the processing operation in terms of involved technology, and can be a way to reuse the processing operation in other processes while someone (e.g. IT department) can change the underlying technology. Method 3 represents the best practice of using dpv:Process to describe all concepts in a modular and granular manner with a separation of concerns. Processes can include other processes - so we can describe processing and technology and data involved as a process and involve it in other processes. This makes the task of finding information easier as we only have to look for composition of processes, instead of investigating each purpose or processing or another concept involved for what data or technology it involves.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0085.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Processing,dpv:hasProcessing,dpv:isImplementedUsingTechnology,dpv:isImplementedByEntity</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -4752,6 +4783,70 @@
         <v>54</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J85" s="9">
+        <v>45658.0</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J86" s="9">
+        <v>45658.0</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4769,22 +4864,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: RISK, Add content to RISK, Add examples
- FIX: RISK potential concepts had a circular reference where they were
declared as instances of themselves e.g. because `PotentialConsequence` was
annotated with role `C` in the spreadsheet. Removing this annotation fixed the
issue.
- Added content to RISK regarding potential concepts as per
https://w3id.org/dpv/meetings/meeting-2025-01-09 including an example showing
the use of potential concepts
- Added example of Rights Impact in RISK (moved existing example in HTML as a
file/concept under UCR)
- Added example of Risk Controls in RISK (earlier example was out of date)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="488">
   <si>
     <t>ID</t>
   </si>
@@ -1424,6 +1424,53 @@
   </si>
   <si>
     <t>dpv:Processing,dpv:hasProcessing,dpv:isImplementedUsingTechnology,dpv:isImplementedByEntity</t>
+  </si>
+  <si>
+    <t>E0086</t>
+  </si>
+  <si>
+    <t>Using Risk Controls to indicate measures adopted for a specific event</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example shows how risk controls can be used to represent the specific measures in place to detect, monitor, address, and inform stakeholders regarding risks, consequences, and impacts. The first part shows a risk with its associated consequence and resulting impact. The second part shows the process where this risk is present, and the specific controls put in place to: (1) monitor the process for vulnerabilities and avoid the source of risk with oversight,; (2) avoid the consequence event; and (3) monitor for occurence of the impact event, and if it occurs to halt it and to inform the affected person.&lt;/p&gt;
+&lt;p&gt;In this example the specific details of the control such as the technology being used, or what characteristics are changed when avoiding an event are not specified to reduce the length of content. To express this information, the specific control can reference two events as Risk and Residual Risk respectively - one which shows the initial values such as likelihood, and another one which shows the modified values. Currently the DPVCG does not dictate a specific method for expressing such information, and welcomes suggestions on best practices for the same.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0086.ttl</t>
+  </si>
+  <si>
+    <t>risk:RiskControl,risk:controls</t>
+  </si>
+  <si>
+    <t>E0087</t>
+  </si>
+  <si>
+    <t>Flexibility of RISK taxonomy in expressing varying roles</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This example shows how the same concept &lt;code&gt;risk:DataBreach&lt;/code&gt; can take on different roles across contexts. The first part shows data breach as a consequence of a malware attack, while the second part shows it as a risk source which could lead to identity fraud and misuse. In these, the same concept of data breach being a consequence or a risk source is context-dependant. The RISK extension does not specify or assert that a data breach is always a risk source or risk or consequence - only that it has the potential to be these things. Therefore, inclusion of RISK extension in the graph does not 'pollute' it or cause misinterpretations such as data breach showing up as a consequence even though it has been asserted to (only) be a risk source.&lt;/p&gt;
+&lt;p&gt;The third part shows how these different roles are associated with the concept, and how this can be used in UI/UX to provide users with a list of options for selecting risks. It also shows the distinction between marking or annotating a concept to include it in risk identification process (&lt;code&gt;risk:PotentialRisk&lt;/code&gt;) and asserting that the concept is applicable as a risk in a process (&lt;code&gt;dpv:hasRisk&lt;/code&gt;). This allows use-cases to directly use the RISK extension's subjective classification of concepts in UI/UX - such as to populate the dropdown of risks, and also provides flexibility to ignore that and create their own thesauri or categorisations by using the &lt;code&gt;risk:PotentialRisk&lt;/code&gt; concept to annotate concepts, or to create specific subclasses for contextual classifications.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>E0087.ttl</t>
+  </si>
+  <si>
+    <t>risk:PotentialRiskSource,risk:PotentialRisk,risk:PotentialConsequence,risk:PotentialImpact</t>
+  </si>
+  <si>
+    <t>E0088</t>
+  </si>
+  <si>
+    <t>Expressing impact on specific rights</t>
+  </si>
+  <si>
+    <t>To express a specific right has been impacted, the relevant rights impact concept is utilised along with a rights impact category from the RISK extension, which together indicate a right is being impacted in the specified manner. In this example, a customer of a company has complained that their GDPR rights have been violated. Upon investigation, it was found that the GDPR's Transparency Right (Article 13) was impacted by limiting the scope of the right as not all processing was represented, and further the right was obstructed as it was not easy to obtain the information on the website.</t>
+  </si>
+  <si>
+    <t>E0088.ttl</t>
+  </si>
+  <si>
+    <t>risk:RightsImpact,eu-gdpr:RightsImpact,risk:RightsViolated,dpv:hasImpact</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -4847,6 +4894,102 @@
         <v>54</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J87" s="9">
+        <v>45669.0</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J88" s="9">
+        <v>45669.0</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J89" s="9">
+        <v>45669.0</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4864,22 +5007,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>467</v>
+        <v>482</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>468</v>
+        <v>483</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>469</v>
+        <v>484</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>471</v>
+        <v>486</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix #318 typos in examples; duplicate in HTML
- Examples (dex) title contained duplicate (x2) titles due to examples
  IRI also being present in other RDF vocabs; solution is to hardcode
  it in the examples jinja2 template as otherwise it requires checking
  for source for each triple and avoiding titles being picked up
- Also fixes typos in example descriptions
    - E0013: criterias -> criteria
    - E0037: orgnisational -> organisational
    - E0069: occured -> occurred
- Fixed typos are also changed in each HTML file the example occurs in

Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ucr.xlsx
+++ b/code/vocab_csv/ucr.xlsx
@@ -344,7 +344,7 @@
   </si>
   <si>
     <t>&lt;p&gt;Consider the use of a spam filter that is based on automated processing operations where humans provide inputs, have oversight of the operation, and results in automated decision making for whether communications should be propagated. A new separate filter is developed that utilises a novel spam detection criteria that also takes into account communications other than emails for the sender and makes automated decisions whether to permit communication to proceed. Such explicit annotation of several high-risk operations assists in performing impact assessments for this technology, as well as understanding the extent and effectiveness of human involvement to mitigate risks and issues.&lt;/p&gt;
-        &lt;p&gt;In this example, the Spam Filter process allows the users to reverse the effects (i.e. emails marked as spam) but does not allow opting out from the process (i.e. stop spam filtering). The spam detection algorithm performs automated decision making (by deciding which emails to accept), systemic monitoring (of communications), and evaluation and scoring (by scoring contents of emails and senders/recipients). The spam detection algorithm also indicates what human involvement is expected - to provide input (e.g. mark emails as spam) and intervention (e.g. change spam criterias).&lt;/p&gt;</t>
+        &lt;p&gt;In this example, the Spam Filter process allows the users to reverse the effects (i.e. emails marked as spam) but does not allow opting out from the process (i.e. stop spam filtering). The spam detection algorithm performs automated decision making (by deciding which emails to accept), systemic monitoring (of communications), and evaluation and scoring (by scoring contents of emails and senders/recipients). The spam detection algorithm also indicates what human involvement is expected - to provide input (e.g. mark emails as spam) and intervention (e.g. change spam criteria).&lt;/p&gt;</t>
   </si>
   <si>
     <t>E0013.ttl</t>
@@ -698,7 +698,7 @@
     <t>E0037</t>
   </si>
   <si>
-    <t>Indicating type of organisation and involvement of specific orgnisational units</t>
+    <t>Indicating type of organisation and involvement of specific organisational units</t>
   </si>
   <si>
     <t>This example involves an organisation that is a NGO, and that it has Marketing, HR, and IT departments. The HR and IT departments are responsible for specific processes.</t>
@@ -1175,7 +1175,7 @@
     <t>Using DPV and RISK extension to represent incidents</t>
   </si>
   <si>
-    <t>This example shows the use of incident concepts in DPV and RISK extension to represent a data breach incident along with its potential and actual (i.e. occured) consequences and impacts on the data subject. It shows the consequences of the incident as loss of data, and which is being misused to cause identity fraud. It also refers to the further risk of financial loss, and associates the incident with a previously identified risk (not elaborated in this example). Note that incident details such as timestamps and durations are not shown in this example.</t>
+    <t>This example shows the use of incident concepts in DPV and RISK extension to represent a data breach incident along with its potential and actual (i.e. occurred) consequences and impacts on the data subject. It shows the consequences of the incident as loss of data, and which is being misused to cause identity fraud. It also refers to the further risk of financial loss, and associates the incident with a previously identified risk (not elaborated in this example). Note that incident details such as timestamps and durations are not shown in this example.</t>
   </si>
   <si>
     <t>E0069.ttl</t>

</xml_diff>